<commit_message>
Update Benchmark Descriptions and Findings.xlsx
</commit_message>
<xml_diff>
--- a/Benchmark Descriptions and Findings.xlsx
+++ b/Benchmark Descriptions and Findings.xlsx
@@ -8,32 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobia\OneDrive\Dokumente\GitHub\MBF_Fidelity_Practitioner09\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490A4FC4-653D-4B9A-94A8-12C1BCDB5BA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C261AA1-F369-40A4-A704-7151EADC071E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{68C3B5FD-8A8D-4046-A25A-1E05F441F067}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Region</t>
   </si>
@@ -44,9 +36,6 @@
     <t>India</t>
   </si>
   <si>
-    <t>Asia Pac ex Japan</t>
-  </si>
-  <si>
     <t>EM Asia</t>
   </si>
   <si>
@@ -74,9 +63,6 @@
     <t>MSCI AC Asia Pac Ex JPN</t>
   </si>
   <si>
-    <t xml:space="preserve">CSI 300 </t>
-  </si>
-  <si>
     <t>IISLN Nifty 50</t>
   </si>
   <si>
@@ -92,14 +78,81 @@
     <t>MSCI EM Asia</t>
   </si>
   <si>
-    <t>CSI Stateowner Enterprises Comp</t>
+    <t>All returns are in U.S. dollars, include dividends and capital gains, and are not continously compounded. Emerging markets currently include Argentina, Brazil, Chile, China, Colombia, Czech Republic, Egypt, Greece, Hungary, India, Indonesia, Malaysia, Mexico, Pakistan, Peru, Philippines, Poland, Qatar, Russia, Saudi Arabia, South Africa, South Korea, Taiwan, Thailand, TUrkey, United Arab Emirates.</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>The MSCI China Index captures large and mid caps representation across China A shares, H shares, B shares, Red chips, P chips and foreihn listings. With 703 constituents, the index covers about 85% of this China equity universe. Currently, the index include Large Cap A and Mid Cap A shares represented at 20% of their free float adjusted market capitalization.</t>
+  </si>
+  <si>
+    <t>CSI 300 Index consists of the largest and most liquid A-share stocks. The Index aims to reflect the overall performance of China A-share market.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constituents are the CSI Local State-Owned Entreprises Index and CSI Central State-Owned Enterprises Composite Index. 
+Local: All A shares are screened by controlliung shareholders. The company is a local state-owned enterprise if finally controlled by local State-owned Assets Supervision and Administration Commission, local municipal goverment and state-owned enterprises. All the local state-owned enterprises listed at Shanghai and Shenzen Stock Exchanges constitute the index.
+</t>
+  </si>
+  <si>
+    <t>The Nifty 50 is the flagship index on the NSE, computed using a float-adjusted, market capitalization weighted methodology. The index tracks the behavior of a portfolio of blue chip companies, the largest and most liquid indian securities dimiciled in India and listed on the NSE.</t>
+  </si>
+  <si>
+    <t>The MSCI India Index is designed to measure the performance of the large and mid cap segements of the Indian equity universe.</t>
+  </si>
+  <si>
+    <t>The S&amp;P BSE India is a free-float weighted index that represents nearly 93% of the total market capitalization on BSE India exchange. This index represents all 20 major industries of the economy.</t>
+  </si>
+  <si>
+    <t>The MSCI AC Asia Pacific ex Japan Index captures large and mid cap representation across 4 of 5 developed markets countries (ex Japan) and 9 Emerging countries in tge Asia Pacific region. With 1,263 constituents, the index covers approx. 85% of the free-float adjusted market cap. in each country.
+DM: Australia, Hong Kong, New Zealand and Singapore.
+EM: China, India, Indonesia, Korea, Malaysia, Pakistan, the Philippines, Taiwan and Thailand</t>
+  </si>
+  <si>
+    <t>Asia PAC</t>
+  </si>
+  <si>
+    <t>The MSCI Emerging Markets (EM) Asia Index captures large and mid cap representation across 9 Emerging Markets countries. With 1,119 constituents, the index covers approximately 85% of the free float-adjusted market capitalization in each country.</t>
+  </si>
+  <si>
+    <t>See below plus 10/40 constraint. Single Issuers cannot be weighted by more than 10% and the companies with weights above 5% cannot have a combined weight of 40%</t>
+  </si>
+  <si>
+    <t>https://www.msci.com/documents/10199/aa99c3a4-d48b-44ac-8caa-49522caa9021</t>
+  </si>
+  <si>
+    <t>http://www.csindex.com.cn/en/indices/index-detail/000300</t>
+  </si>
+  <si>
+    <t>http://www.csindex.com.cn/old_notices/en</t>
+  </si>
+  <si>
+    <t>https://www.bloomberg.com/quote/NIFTY:IND</t>
+  </si>
+  <si>
+    <t>https://www.msci.com/documents/10199/1ad792ce-3199-445c-8be3-f2a035ac782d</t>
+  </si>
+  <si>
+    <t>https://www.msci.com/documents/10199/0df2ed3c-5fea-4414-b875-55dcd31705ad</t>
+  </si>
+  <si>
+    <t>https://www.bloomberg.com/quote/BSE500:IND</t>
+  </si>
+  <si>
+    <t>https://www.msci.com/documents/10199/17e9365e-fbf6-407e-9f48-808f7b75a5bf</t>
+  </si>
+  <si>
+    <t>JavaScript must be enabled.</t>
+  </si>
+  <si>
+    <t>https://mba.tuck.dartmouth.edu/pages/faculty/ken.french/Data_Library/f-f_5emerging.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +163,20 @@
     <font>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF24292E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -156,26 +223,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -487,146 +564,192 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08F90FE-C225-4BE0-B9EB-7B028112B575}">
-  <dimension ref="A1:E18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.08984375" customWidth="1"/>
-    <col min="3" max="3" width="27.08984375" customWidth="1"/>
-    <col min="4" max="4" width="48.453125" customWidth="1"/>
-    <col min="5" max="5" width="37.453125" customWidth="1"/>
+    <col min="1" max="1" width="35.7265625" customWidth="1"/>
+    <col min="3" max="3" width="27.1796875" customWidth="1"/>
+    <col min="4" max="4" width="71.81640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="37.453125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="32.26953125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:6" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+    </row>
+    <row r="3" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
+      <c r="D3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9"/>
       <c r="C4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
+      <c r="D4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4"/>
+    </row>
+    <row r="5" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="9"/>
       <c r="C5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
+      <c r="D5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="7"/>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7"/>
+    </row>
+    <row r="8" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="7"/>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="7"/>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="C9" t="s">
+      <c r="D10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10"/>
+    </row>
+    <row r="11" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="C10" t="s">
+      <c r="D11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="8"/>
+      <c r="C12" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="3"/>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="3"/>
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="3"/>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="4"/>
-      <c r="C16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="4"/>
-      <c r="C17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="4"/>
-      <c r="C18" t="s">
-        <v>19</v>
+      <c r="D12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E19" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A18"/>
+  <mergeCells count="3">
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A3:A5"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
trying out stuff, creating rmd, adding findings to excel
</commit_message>
<xml_diff>
--- a/Benchmark Descriptions and Findings.xlsx
+++ b/Benchmark Descriptions and Findings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobia\OneDrive\Dokumente\GitHub\MBF_Fidelity_Practitioner09\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C261AA1-F369-40A4-A704-7151EADC071E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FCC47D-F12C-4242-B006-3B335D035978}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
   <si>
     <t>Region</t>
   </si>
@@ -142,10 +142,56 @@
     <t>https://www.msci.com/documents/10199/17e9365e-fbf6-407e-9f48-808f7b75a5bf</t>
   </si>
   <si>
-    <t>JavaScript must be enabled.</t>
-  </si>
-  <si>
     <t>https://mba.tuck.dartmouth.edu/pages/faculty/ken.french/Data_Library/f-f_5emerging.html</t>
+  </si>
+  <si>
+    <t>10y and 5y: Funds underperform in the CAPM, but outperform in the 4- and 5-factor model.
+3y: Funds outperform in every model except the Carhart model, where they underperform.</t>
+  </si>
+  <si>
+    <t>Funds outperform in every time horizon and every factor model. Alphas beween 20bp and 48bp. Stronger performance recently.</t>
+  </si>
+  <si>
+    <t>Small but significant outperformance in 1- and 3- factor model. Higher outperformance  around 30bp in 4- and 5-factor model. Consistent over time.</t>
+  </si>
+  <si>
+    <t>Funds outperform in every time horizon and every factor model. Huge alphas, especially in the last three years. (90bp p.m.!!!)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10y: Underperformance in CAPM, Outperformance in 4- and 5-factor model
+3 and 5y: Mixed, but significant results </t>
+  </si>
+  <si>
+    <t>Strong outperformance for each time horizon. Decreased recent outperformance in five factor model.</t>
+  </si>
+  <si>
+    <t>Small but significant underperformance in each model and each time horizon.</t>
+  </si>
+  <si>
+    <t>Strong outperformance in each model and each time horizon. Outperformance recently higher for low factor models.</t>
+  </si>
+  <si>
+    <t>3y and 5y: underperformance in four factor models. 
+10y  overperformance in higher factor models.</t>
+  </si>
+  <si>
+    <t>Consistent underperformance in every factor model and time horizon.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3y and 5y: underperformance in every factor model
+10y:  negative alphas, sometimes significantly
+</t>
+  </si>
+  <si>
+    <t>Small and sometimes significant underperformance in each model and each time horizon, especially in lower factor models.</t>
+  </si>
+  <si>
+    <t>Strong and significant outperformance in most time and factor specifications.</t>
+  </si>
+  <si>
+    <t>3y: No significant alphas except 4 factor model underperforms
+5y: Mostly underperformance except in 4 facto model in which funds overperform
+10y: Underperformance in CAPM, strong performance in 5 factor model</t>
   </si>
 </sst>
 </file>
@@ -229,9 +275,6 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -248,6 +291,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -565,35 +611,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="69" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="35.7265625" customWidth="1"/>
     <col min="3" max="3" width="27.1796875" customWidth="1"/>
-    <col min="4" max="4" width="71.81640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="37.453125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="32.26953125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="71.81640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="37.453125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="32.26953125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -602,152 +648,251 @@
       <c r="E2"/>
       <c r="F2"/>
     </row>
-    <row r="3" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:6" ht="106.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3"/>
+    </row>
+    <row r="4" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="8"/>
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="9"/>
-      <c r="C4" t="s">
+    <row r="5" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="8"/>
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F4"/>
-    </row>
-    <row r="5" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="9"/>
-      <c r="C5" t="s">
+    </row>
+    <row r="6" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="8"/>
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
+    </row>
+    <row r="7" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="7"/>
-      <c r="C7" t="s">
+      <c r="E7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="6"/>
+      <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F7"/>
-    </row>
-    <row r="8" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="7"/>
-      <c r="C8" t="s">
+    </row>
+    <row r="9" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="6"/>
+      <c r="C9" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="7"/>
-      <c r="C9" t="s">
+    </row>
+    <row r="10" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="6"/>
+      <c r="C10" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="9"/>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="9"/>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="9"/>
+      <c r="C14" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F10"/>
-    </row>
-    <row r="11" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="8" t="s">
+    </row>
+    <row r="15" spans="1:6" ht="104" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C15" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="8"/>
-      <c r="C12" t="s">
+      <c r="E15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" ht="104" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="7"/>
+      <c r="C16" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E19" t="s">
-        <v>37</v>
-      </c>
+    <row r="17" spans="1:5" ht="104" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="7"/>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="104" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="7"/>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E23"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A3:A5"/>
+  <mergeCells count="4">
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A18"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>